<commit_message>
Initial missing file exception fix
</commit_message>
<xml_diff>
--- a/src/xlsxtocsv/MasterPriceFile_v4.xlsx
+++ b/src/xlsxtocsv/MasterPriceFile_v4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>New</t>
   </si>
@@ -229,6 +229,15 @@
   </si>
   <si>
     <t>CarryOver</t>
+  </si>
+  <si>
+    <t>SPORTSW</t>
+  </si>
+  <si>
+    <t>AGDISC</t>
+  </si>
+  <si>
+    <t>CROWN</t>
   </si>
 </sst>
 </file>
@@ -567,9 +576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -592,7 +603,7 @@
     <col min="18" max="18" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,8 +658,17 @@
       <c r="R1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>95000</v>
       </c>
@@ -700,8 +720,17 @@
       <c r="R2">
         <v>130.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S2">
+        <v>130.5</v>
+      </c>
+      <c r="T2">
+        <v>126.15</v>
+      </c>
+      <c r="U2">
+        <v>130.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>95001</v>
       </c>
@@ -753,8 +782,17 @@
       <c r="R3">
         <v>92.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S3">
+        <v>92.25</v>
+      </c>
+      <c r="T3">
+        <v>89.18</v>
+      </c>
+      <c r="U3">
+        <v>92.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -809,8 +847,17 @@
       <c r="R4">
         <v>95.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S4">
+        <v>95.4</v>
+      </c>
+      <c r="T4">
+        <v>92.22</v>
+      </c>
+      <c r="U4">
+        <v>95.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>95279</v>
       </c>
@@ -865,8 +912,17 @@
       <c r="R5">
         <v>86.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S5">
+        <v>86.4</v>
+      </c>
+      <c r="T5">
+        <v>83.52</v>
+      </c>
+      <c r="U5">
+        <v>86.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>95065</v>
       </c>
@@ -918,8 +974,17 @@
       <c r="R6">
         <v>76.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6">
+        <v>76.5</v>
+      </c>
+      <c r="T6">
+        <v>73.95</v>
+      </c>
+      <c r="U6">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -974,8 +1039,17 @@
       <c r="R7">
         <v>64.350000000000009</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S7">
+        <v>64.349999999999994</v>
+      </c>
+      <c r="T7">
+        <v>62.21</v>
+      </c>
+      <c r="U7">
+        <v>64.349999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1030,8 +1104,17 @@
       <c r="R8">
         <v>61.92</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S8">
+        <v>61.92</v>
+      </c>
+      <c r="T8">
+        <v>59.86</v>
+      </c>
+      <c r="U8">
+        <v>61.92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>95646</v>
       </c>
@@ -1083,8 +1166,17 @@
       <c r="R9">
         <v>42.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9">
+        <v>42.75</v>
+      </c>
+      <c r="T9">
+        <v>41.33</v>
+      </c>
+      <c r="U9">
+        <v>42.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>31</v>
       </c>
@@ -1136,8 +1228,17 @@
       <c r="R10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>95007</v>
       </c>
@@ -1189,8 +1290,17 @@
       <c r="R11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1245,8 +1355,17 @@
       <c r="R12">
         <v>53.550000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12">
+        <v>53.55</v>
+      </c>
+      <c r="T12">
+        <v>51.77</v>
+      </c>
+      <c r="U12">
+        <v>53.55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1298,8 +1417,17 @@
       <c r="R13">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S13">
+        <v>54</v>
+      </c>
+      <c r="T13">
+        <v>52.2</v>
+      </c>
+      <c r="U13">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1351,8 +1479,17 @@
       <c r="R14">
         <v>47.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14">
+        <v>47.25</v>
+      </c>
+      <c r="T14">
+        <v>45.68</v>
+      </c>
+      <c r="U14">
+        <v>47.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1407,8 +1544,17 @@
       <c r="R15">
         <v>41.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S15">
+        <v>41.4</v>
+      </c>
+      <c r="T15">
+        <v>40.020000000000003</v>
+      </c>
+      <c r="U15">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>43</v>
       </c>
@@ -1460,8 +1606,17 @@
       <c r="R16">
         <v>25.650000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S16">
+        <v>25.65</v>
+      </c>
+      <c r="T16">
+        <v>24.8</v>
+      </c>
+      <c r="U16">
+        <v>25.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>45</v>
       </c>
@@ -1513,8 +1668,17 @@
       <c r="R17">
         <v>18.900000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S17">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="T17">
+        <v>18.27</v>
+      </c>
+      <c r="U17">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1566,8 +1730,17 @@
       <c r="R18">
         <v>33.75</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S18">
+        <v>33.75</v>
+      </c>
+      <c r="T18">
+        <v>32.630000000000003</v>
+      </c>
+      <c r="U18">
+        <v>33.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1619,8 +1792,17 @@
       <c r="R19">
         <v>30.150000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S19">
+        <v>30.15</v>
+      </c>
+      <c r="T19">
+        <v>29.15</v>
+      </c>
+      <c r="U19">
+        <v>30.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1672,8 +1854,17 @@
       <c r="R20">
         <v>23.400000000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S20">
+        <v>23.4</v>
+      </c>
+      <c r="T20">
+        <v>22.62</v>
+      </c>
+      <c r="U20">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1725,8 +1916,17 @@
       <c r="R21">
         <v>23.400000000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S21">
+        <v>23.4</v>
+      </c>
+      <c r="T21">
+        <v>22.62</v>
+      </c>
+      <c r="U21">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -1778,8 +1978,17 @@
       <c r="R22">
         <v>20.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S22">
+        <v>20.7</v>
+      </c>
+      <c r="T22">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="U22">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1831,8 +2040,17 @@
       <c r="R23">
         <v>20.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S23">
+        <v>20.7</v>
+      </c>
+      <c r="T23">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="U23">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1884,8 +2102,17 @@
       <c r="R24">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S24">
+        <v>27</v>
+      </c>
+      <c r="T24">
+        <v>26.1</v>
+      </c>
+      <c r="U24">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -1937,8 +2164,17 @@
       <c r="R25">
         <v>64.350000000000009</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S25">
+        <v>64.349999999999994</v>
+      </c>
+      <c r="T25">
+        <v>62.21</v>
+      </c>
+      <c r="U25">
+        <v>64.349999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>94320</v>
       </c>
@@ -1993,8 +2229,17 @@
       <c r="R26">
         <v>42.75</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S26">
+        <v>42.75</v>
+      </c>
+      <c r="T26">
+        <v>41.33</v>
+      </c>
+      <c r="U26">
+        <v>42.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>94445</v>
       </c>
@@ -2046,8 +2291,17 @@
       <c r="R27">
         <v>25.650000000000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S27">
+        <v>25.65</v>
+      </c>
+      <c r="T27">
+        <v>24.8</v>
+      </c>
+      <c r="U27">
+        <v>25.65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>94456</v>
       </c>
@@ -2099,8 +2353,17 @@
       <c r="R28">
         <v>18.900000000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S28">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="T28">
+        <v>18.27</v>
+      </c>
+      <c r="U28">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -2152,8 +2415,17 @@
       <c r="R29">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S29">
+        <v>45</v>
+      </c>
+      <c r="T29">
+        <v>43.5</v>
+      </c>
+      <c r="U29">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -2203,6 +2475,15 @@
         <v>36</v>
       </c>
       <c r="R30">
+        <v>36</v>
+      </c>
+      <c r="S30">
+        <v>36</v>
+      </c>
+      <c r="T30">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="U30">
         <v>36</v>
       </c>
     </row>

</xml_diff>